<commit_message>
Update version, preparing for pre-release testing.
</commit_message>
<xml_diff>
--- a/Example/MasterScriptTemplate.xlsx
+++ b/Example/MasterScriptTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>_MasterItemType</t>
   </si>
@@ -105,6 +105,39 @@
   </si>
   <si>
     <t>dim;tag1;another</t>
+  </si>
+  <si>
+    <t>_MasterItemID</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Super Drill Down</t>
+  </si>
+  <si>
+    <t>This drills down through 5 levels</t>
+  </si>
+  <si>
+    <t>dim;super;tags</t>
+  </si>
+  <si>
+    <t>Dim3</t>
+  </si>
+  <si>
+    <t>AsciiAlpha</t>
+  </si>
+  <si>
+    <t>AsciiNum</t>
   </si>
 </sst>
 </file>
@@ -465,114 +498,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue where required 5 Expression fields. Now works with dynamic list as designed.
Version 1.0.1
</commit_message>
<xml_diff>
--- a/Example/MasterScriptTemplate.xlsx
+++ b/Example/MasterScriptTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>_MasterItemType</t>
   </si>
@@ -108,18 +108,6 @@
   </si>
   <si>
     <t>_MasterItemID</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D3</t>
   </si>
   <si>
     <t>Super Drill Down</t>
@@ -501,7 +489,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,8 +538,8 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
+      <c r="A2">
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -573,8 +561,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
+      <c r="A3">
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -596,8 +584,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
+      <c r="A4">
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -622,20 +610,20 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
+      <c r="A5">
+        <v>104</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -644,13 +632,13 @@
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue where would break when using HidePrefix Maximises the number of rows that can be imported to use full hypercube size
</commit_message>
<xml_diff>
--- a/Example/MasterScriptTemplate.xlsx
+++ b/Example/MasterScriptTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="47925" windowHeight="17610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="6510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,9 +500,11 @@
     <col min="4" max="4" width="24.85546875" customWidth="1"/>
     <col min="5" max="6" width="24.42578125" customWidth="1"/>
     <col min="7" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -536,8 +538,10 @@
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101</v>
       </c>
@@ -560,7 +564,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>102</v>
       </c>
@@ -583,7 +587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>103</v>
       </c>
@@ -609,7 +613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
Updated to support September 2017 Label Expressions.
</commit_message>
<xml_diff>
--- a/Example/MasterScriptTemplate.xlsx
+++ b/Example/MasterScriptTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>_MasterItemType</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>AsciiNum</t>
+  </si>
+  <si>
+    <t>_MasterItemLabel</t>
+  </si>
+  <si>
+    <t>GetSelectedCount(Alpha)</t>
+  </si>
+  <si>
+    <t>Dim Name Here!</t>
   </si>
 </sst>
 </file>
@@ -489,7 +498,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +547,9 @@
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -586,6 +597,9 @@
       <c r="G3" t="s">
         <v>18</v>
       </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -643,6 +657,9 @@
       </c>
       <c r="K5" t="s">
         <v>33</v>
+      </c>
+      <c r="L5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to Fix issue with no color on measures.
Release 1.1.1
</commit_message>
<xml_diff>
--- a/Example/MasterScriptTemplate.xlsx
+++ b/Example/MasterScriptTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>_MasterItemType</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>This is Measure 1 created from data</t>
-  </si>
-  <si>
-    <t>#00ff00</t>
   </si>
   <si>
     <t>sum(Num)</t>
@@ -497,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +512,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -530,7 +527,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -548,7 +545,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M1" s="1"/>
     </row>
@@ -569,7 +566,7 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -588,17 +585,14 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -609,22 +603,22 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -635,31 +629,31 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>31</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>32</v>
       </c>
-      <c r="K5" t="s">
-        <v>33</v>
-      </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to support June 2018 Release
</commit_message>
<xml_diff>
--- a/Example/MasterScriptTemplate.xlsx
+++ b/Example/MasterScriptTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>_MasterItemType</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>GetSelectedCount(Alpha)</t>
-  </si>
-  <si>
-    <t>Dim Name Here!</t>
   </si>
 </sst>
 </file>
@@ -494,16 +491,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
     <col min="5" max="6" width="24.42578125" customWidth="1"/>
     <col min="7" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.85546875" customWidth="1"/>
@@ -652,9 +649,6 @@
       <c r="K5" t="s">
         <v>32</v>
       </c>
-      <c r="L5" t="s">
-        <v>35</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>